<commit_message>
Upgrading data extraction, logs and parsing.
</commit_message>
<xml_diff>
--- a/recibo.xlsx
+++ b/recibo.xlsx
@@ -16,8 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,13 +30,22 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004F81BD"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,11 +66,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -434,9 +446,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="50" customWidth="1" min="4" max="4"/>
+    <col width="40" customWidth="1" min="4" max="4"/>
     <col width="80" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
@@ -470,91 +482,58 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>25/05/0023</t>
+          <t>26/06/2025</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Pe Pe ee at</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
+          <t>MEGA FRUVER EL SUPEF</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>TOTAL NO ENCONTRADO</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ane Soren $13,990
-NIT: 890.319, 193-3</t>
+          <t>0.59</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Pe Pe ee at
-encod
-Cree
-Simei brane ‘i
-Pee oC en ed
-Sari MCI ea
-Ca ea AL
-Bee en Cee
-Pac AA
-CER Laas
-A Tr RE
-CT ae ae) Piste LL
-FMI 11, ke
-ee ee ear. cea
-Pee re tar
-eran
-Bran Wate mea bg
-prc
-eee Re (sea Ua
-PE eee ee
-era Hepa)
-PTC Rae)
-Tite ST
-Direccion :
-Oa
-Ce na i
-a U
-MOM UAE ES na Oc
-Sm) 13890 13990
-ane Soren $13,990
-Cg ao i
-eee a a, Cat ee eee
-eee a rns ry
-aan) coon
-eT ena
-AUC e Lec anc)
-No, 18764093481383
-Pees
-Pe ce Rec ue)
-Vigencia: desde 2025/05/23
-aie eS)
-Ree UU
-[iss MM rma eee ad
-CEE amen aL)
-rie U gL Lae)
-Prt ea ar)
-Factura ganarada por software de
-Sg rac er aa
-NIT: 890.319, 193-3
-Aa wa)
-lig
-Eee Te Ue eee TEE
-CURA eee kn Tt)
-Coie)
-eae Cy
-Fe am cacey ED)
-Ohya eae y
-Ee
-Car ae
-ZT ne
-pee sc
-fore eon
-Ren eh eee
-Per aa</t>
+          <t>Espacio para
+; Logo Corporativo
+MEGA FRUVER EL SUPEF
+REGALON SAS
+Le
+Dir.: CALLE 8 26 - 17 |
+rE ISA ies
+Documento de ingreso
+PMP AL Yd
+er Cle 26/06/2025, 11 35
+CMe Cr AO RE eT BC Reems
+NaC M TMC Ne Cat alk 1 eke 1a ee
+soporte de uso cantable
+ety Consumidor Final
+C.c i NIT: 222222222222-7
+ital
+Vendedor: jhon anderson arango
+| or ZT)
+0.59
+4 yt) RATA) PAR,
+PAPA AMARIILA GRANEL / 3001
+ce
+2 ts Pe oPoUeR
+LIMON TAHITI / 1017
+E pK y
+3 mT ALOK) SSK
+es San ad
+‘. are
+C224.)
+Ae)
+Rend
+ray</t>
         </is>
       </c>
     </row>

</xml_diff>